<commit_message>
nuevas restricciones y arreglos para solucionar errores
</commit_message>
<xml_diff>
--- a/data/datos_min.xlsx
+++ b/data/datos_min.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\flexible-vrp\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFG\flexible-vrp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34050979-9D98-48C5-96BA-16A038284DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7734FC-CB17-4FC6-B006-F47EFFD7AE05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -521,16 +521,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -538,7 +538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -546,7 +546,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -554,7 +554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -562,7 +562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -570,7 +570,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -578,7 +578,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -586,7 +586,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -594,7 +594,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -602,7 +602,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -624,9 +624,9 @@
       <selection activeCell="A3" sqref="A3:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -637,7 +637,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -648,7 +648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -659,7 +659,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -670,7 +670,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -681,7 +681,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -692,7 +692,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -703,7 +703,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -714,7 +714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -725,7 +725,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -736,7 +736,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -747,7 +747,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -758,7 +758,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -769,7 +769,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -780,7 +780,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -791,7 +791,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -802,7 +802,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -813,7 +813,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -824,7 +824,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -835,7 +835,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -846,7 +846,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -857,7 +857,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -868,7 +868,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -879,7 +879,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -890,7 +890,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -901,7 +901,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -912,7 +912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -923,7 +923,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -934,7 +934,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -945,7 +945,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -956,7 +956,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -967,7 +967,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -978,7 +978,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -989,7 +989,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>16</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>17</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>17</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>18</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>18</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>18</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>18</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -1263,13 +1263,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1291,35 +1291,35 @@
         <v>15</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C3">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C4">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D4">
         <v>0</v>

</xml_diff>

<commit_message>
c1 modificada para incluir todas las paradas
</commit_message>
<xml_diff>
--- a/data/datos_min.xlsx
+++ b/data/datos_min.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\flexible-vrp\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Mi unidad\academico\docencia\tfx\en_curso\stn\codigo\flexible-vrp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC97240-AB8E-415E-B58F-C8431978E32E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D551CE38-530B-4495-8141-91D444421294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="26">
   <si>
     <t>name</t>
   </si>
@@ -521,7 +521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -551,7 +551,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1261,10 +1261,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1285,43 +1285,15 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C2">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4">
-        <v>26</v>
-      </c>
-      <c r="D4">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ordenamos, añadimos una restricción y commodities
</commit_message>
<xml_diff>
--- a/data/datos_min.xlsx
+++ b/data/datos_min.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFG\flexible-vrp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC97B481-4C90-423D-A34C-B097EA7F268E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717C59E0-0313-4AAD-95E0-A3215EECCD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="1365" windowWidth="15375" windowHeight="9180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6750" yWindow="1755" windowWidth="15375" windowHeight="9180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="26">
   <si>
     <t>name</t>
   </si>
@@ -1274,10 +1274,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1338,6 +1338,62 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>143</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>28</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>91</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>